<commit_message>
Updated with next idaithalam version 1.6.1
</commit_message>
<xml_diff>
--- a/demo-all/src/test/resources/rest/demo-all.xlsx
+++ b/demo-all/src/test/resources/rest/demo-all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\feb-release\microservices-lowcode-testautomation\demo-all\src\test\resources\rest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B86CD4-BE32-4811-967A-AEBE83DC923F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96ECDAB4-C364-4621-BADE-37FBCDFD633D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
@@ -944,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E57E3D-0C14-46A6-9520-2A3B86BE3763}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,7 +1119,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>